<commit_message>
Added new components to BOM for sensor assembly
</commit_message>
<xml_diff>
--- a/Track Parts/Starting Gate with Timer/Bill of Materials - Start Gate.xlsx
+++ b/Track Parts/Starting Gate with Timer/Bill of Materials - Start Gate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
   <si>
     <t>Required for</t>
   </si>
@@ -590,17 +590,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="97.7109375" bestFit="1" customWidth="1"/>
@@ -831,7 +831,7 @@
         <v>6</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
         <v>46</v>
@@ -969,7 +969,7 @@
         <v>11</v>
       </c>
       <c r="B21">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
         <v>63</v>
@@ -983,7 +983,7 @@
         <v>11</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
         <v>67</v>
@@ -998,6 +998,71 @@
       </c>
       <c r="C23" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1008,8 +1073,8 @@
     <hyperlink ref="F6" r:id="rId4"/>
     <hyperlink ref="F8" r:id="rId5"/>
     <hyperlink ref="F9" r:id="rId6"/>
-    <hyperlink ref="F10"/>
-    <hyperlink ref="F4"/>
+    <hyperlink ref="F10" display="https://www.amazon.com/Willwin-Female-Accessories-Connector-Adaptor/dp/B074QGFDM8/ref=sr_1_7_sspa?crid=4TJRCFDRAYB1&amp;dchild=1&amp;keywords=db9%2Bconnector&amp;qid=1596222297&amp;sprefix=DB9%2Caps%2C171&amp;sr=8-7-spons&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzS084M1pCTUZXNkRFJmVu"/>
+    <hyperlink ref="F4" display="https://www.amazon.com/Willwin-Female-Accessories-Connector-Adaptor/dp/B074QGFDM8/ref=sr_1_7_sspa?crid=4TJRCFDRAYB1&amp;dchild=1&amp;keywords=db9%2Bconnector&amp;qid=1596222297&amp;sprefix=DB9%2Caps%2C171&amp;sr=8-7-spons&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzS084M1pCTUZXNkRFJmVu"/>
     <hyperlink ref="F5" r:id="rId7"/>
     <hyperlink ref="F12" r:id="rId8" display="https://www.amazon.com/Female-Extension-RS232-Serial-Cable/dp/B06XTD479F/ref=sr_1_1_sspa?dchild=1&amp;keywords=DB9%2Bcable&amp;qid=1596223468&amp;sr=8-1-spons&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUE4SzYzTDhJSVZMM0smZW5jcnlwdGVkSWQ9QTA0MTE3MjM4STVES0xMVU9FQkImZW5jcnlwdGVkQWRJZD1BMDU4MjE4MzNOTFExSFQyRVNHNTImd2lkZ2V0TmFtZT1zcF9hdGYmYWN0aW9uPWNsaWNrUmVkaXJlY3QmZG9Ob3RMb2dDbGljaz10cnVl&amp;th=1"/>
     <hyperlink ref="F13" r:id="rId9"/>
@@ -1018,9 +1083,12 @@
     <hyperlink ref="F11" r:id="rId12"/>
     <hyperlink ref="F17" r:id="rId13"/>
     <hyperlink ref="F21" r:id="rId14"/>
+    <hyperlink ref="F24" display="https://www.amazon.com/Willwin-Female-Accessories-Connector-Adaptor/dp/B074QGFDM8/ref=sr_1_7_sspa?crid=4TJRCFDRAYB1&amp;dchild=1&amp;keywords=db9%2Bconnector&amp;qid=1596222297&amp;sprefix=DB9%2Caps%2C171&amp;sr=8-7-spons&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzS084M1pCTUZXNkRFJmVu"/>
+    <hyperlink ref="F25" display="https://www.amazon.com/Willwin-Female-Accessories-Connector-Adaptor/dp/B074QGFDM8/ref=sr_1_7_sspa?crid=4TJRCFDRAYB1&amp;dchild=1&amp;keywords=db9%2Bconnector&amp;qid=1596222297&amp;sprefix=DB9%2Caps%2C171&amp;sr=8-7-spons&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzS084M1pCTUZXNkRFJmVu"/>
+    <hyperlink ref="F26" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update Bill of Materials - Start Gate.xlsx
Added self tapping screws to BOM
</commit_message>
<xml_diff>
--- a/Track Parts/Starting Gate with Timer/Bill of Materials - Start Gate.xlsx
+++ b/Track Parts/Starting Gate with Timer/Bill of Materials - Start Gate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="74">
   <si>
     <t>Required for</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>https://www.mcmaster.com/95117A499/</t>
+  </si>
+  <si>
+    <t>#4 - 18-8 5/16" Self Tapping Screw</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/90065A107/</t>
   </si>
 </sst>
 </file>
@@ -590,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,6 +1069,20 @@
       </c>
       <c r="C27" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1086,9 +1106,10 @@
     <hyperlink ref="F24" display="https://www.amazon.com/Willwin-Female-Accessories-Connector-Adaptor/dp/B074QGFDM8/ref=sr_1_7_sspa?crid=4TJRCFDRAYB1&amp;dchild=1&amp;keywords=db9%2Bconnector&amp;qid=1596222297&amp;sprefix=DB9%2Caps%2C171&amp;sr=8-7-spons&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzS084M1pCTUZXNkRFJmVu"/>
     <hyperlink ref="F25" display="https://www.amazon.com/Willwin-Female-Accessories-Connector-Adaptor/dp/B074QGFDM8/ref=sr_1_7_sspa?crid=4TJRCFDRAYB1&amp;dchild=1&amp;keywords=db9%2Bconnector&amp;qid=1596222297&amp;sprefix=DB9%2Caps%2C171&amp;sr=8-7-spons&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzS084M1pCTUZXNkRFJmVu"/>
     <hyperlink ref="F26" r:id="rId15"/>
+    <hyperlink ref="F28" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>